<commit_message>
Change policy indicators to CDC's suggestions from 11/10/2022. Removed continuous and dummy indicators calculated on quartiles. Only dummy indicators for CDC suggestions remain. 05modeling.r is almost complete.
</commit_message>
<xml_diff>
--- a/district_policy_items.xlsx
+++ b/district_policy_items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icfonline-my.sharepoint.com/personal/53643_icf_com/Documents/Work/work_2022/nscps_district_cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7183EF97-0A10-7C41-8997-32384100B94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="8_{7183EF97-0A10-7C41-8997-32384100B94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67D7FD2D-887D-A34B-861E-F592D60E1CF0}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="20220" windowHeight="17440" xr2:uid="{F918339D-8002-A648-9553-BC048C0A423A}"/>
+    <workbookView xWindow="2520" yWindow="3200" windowWidth="27180" windowHeight="17440" xr2:uid="{F918339D-8002-A648-9553-BC048C0A423A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="63">
   <si>
     <t>Offer paid leave for teachers and staff who have side effects from vaccine</t>
   </si>
@@ -191,10 +191,40 @@
     <t>Cleaning</t>
   </si>
   <si>
-    <t>Trace and Quarantine</t>
-  </si>
-  <si>
     <t>Ventilation</t>
+  </si>
+  <si>
+    <t>cdc</t>
+  </si>
+  <si>
+    <t>operation</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>Contact tracing</t>
+  </si>
+  <si>
+    <t>Quarantine</t>
+  </si>
+  <si>
+    <t>HVAC systems</t>
+  </si>
+  <si>
+    <t>HEPA filters</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>score_needed</t>
+  </si>
+  <si>
+    <t>either</t>
+  </si>
+  <si>
+    <t>Screening testing for students</t>
   </si>
 </sst>
 </file>
@@ -288,6 +318,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -587,351 +621,643 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19F5AF8C-B985-6A4A-BF29-A5E5F97C4F2C}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="90" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>41</v>
       </c>
       <c r="B1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>54</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B35" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>54</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>54</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>52</v>
+        <v>57</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>54</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalized analyses. Lots of adjustments.
</commit_message>
<xml_diff>
--- a/district_policy_items.xlsx
+++ b/district_policy_items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icfonline-my.sharepoint.com/personal/53643_icf_com/Documents/Work/work_2022/nscps_district_cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="8_{7183EF97-0A10-7C41-8997-32384100B94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67D7FD2D-887D-A34B-861E-F592D60E1CF0}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="8_{7183EF97-0A10-7C41-8997-32384100B94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC66523A-BFAA-6045-88C9-3D9DE8E3262C}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="3200" windowWidth="27180" windowHeight="17440" xr2:uid="{F918339D-8002-A648-9553-BC048C0A423A}"/>
+    <workbookView xWindow="660" yWindow="3200" windowWidth="13400" windowHeight="17440" xr2:uid="{F918339D-8002-A648-9553-BC048C0A423A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,12 +47,6 @@
     <t>Offer to host information sessions to connect families with information about vaccinations</t>
   </si>
   <si>
-    <t>Offer vaccines at district sponsored events to teachers and staff</t>
-  </si>
-  <si>
-    <t>Offer vaccines at district sponsored events to eligible students</t>
-  </si>
-  <si>
     <t>Offer vaccines at district sponsored events to families andor community members</t>
   </si>
   <si>
@@ -110,9 +104,6 @@
     <t>Offer or support the screening testing of teachers and staff on a regular basis</t>
   </si>
   <si>
-    <t>Offer or support the screening testing of students on a regular basis</t>
-  </si>
-  <si>
     <t>Offer paid sick leave for teachers and staff who are sick</t>
   </si>
   <si>
@@ -134,9 +125,6 @@
     <t>Teachers and staff quarantine if identified to be a close contact</t>
   </si>
   <si>
-    <t>Students quarantine if identified to be a close contact</t>
-  </si>
-  <si>
     <t>Disinfect spaces that have been occupied by a person who is sick or has tested positive for COVID-19</t>
   </si>
   <si>
@@ -158,9 +146,6 @@
     <t>Use high-efficiency particulate air (HEPA) filters</t>
   </si>
   <si>
-    <t>Replace, upgrade, maintain, or inspect HVAC systems</t>
-  </si>
-  <si>
     <t>Item</t>
   </si>
   <si>
@@ -225,6 +210,21 @@
   </si>
   <si>
     <t>Screening testing for students</t>
+  </si>
+  <si>
+    <t>Offer COVID-19 vaccines at district sponsored events to teachers and staff</t>
+  </si>
+  <si>
+    <t>Offer COVID-19 vaccines at district sponsored events to eligible students</t>
+  </si>
+  <si>
+    <t>Offer or support COVID-19 screening testing of students on a regular basis</t>
+  </si>
+  <si>
+    <t>Replace, upgrade, maintain, or inspect heating, ventilation, and air conditioning (HVAC) systems</t>
+  </si>
+  <si>
+    <t>Students quarantine if identified as a close contact</t>
   </si>
 </sst>
 </file>
@@ -623,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19F5AF8C-B985-6A4A-BF29-A5E5F97C4F2C}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -635,544 +635,550 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>56</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>56</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
         <v>54</v>
-      </c>
-      <c r="E15">
-        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="B29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="B30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="B31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="B32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="B33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="B34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>54</v>
-      </c>
-      <c r="E26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-      <c r="D27" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B29" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>54</v>
-      </c>
-      <c r="E30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31" t="s">
-        <v>54</v>
-      </c>
-      <c r="E31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" t="s">
-        <v>56</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34" t="s">
-        <v>54</v>
-      </c>
-      <c r="E34">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>50</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D36" t="s">
         <v>54</v>
       </c>
-      <c r="E36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B37" t="s">
         <v>51</v>
@@ -1181,86 +1187,83 @@
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B38" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B39" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B41" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41" t="s">
         <v>54</v>
       </c>
-      <c r="E41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B42" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D42" t="s">
         <v>54</v>
       </c>
-      <c r="E42">
-        <v>2</v>
-      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E42">
+    <sortCondition descending="1" ref="C2:C42"/>
+  </sortState>
   <conditionalFormatting sqref="A2:A42">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(),2)=0</formula>

</xml_diff>